<commit_message>
Fixes to Langtjern input files
</commit_message>
<xml_diff>
--- a/LangtjernLake/ConfigurationInputsLangtjern.xlsx
+++ b/LangtjernLake/ConfigurationInputsLangtjern.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\SOS\LangtjernLake\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10116" windowHeight="4140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10110" windowHeight="4140"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -441,7 +436,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -449,15 +444,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,12 +463,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -484,7 +479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -495,7 +490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -506,7 +501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -517,7 +512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -528,7 +523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -539,12 +534,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -555,12 +550,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -571,7 +566,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -582,7 +577,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -593,7 +588,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -604,7 +599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -615,7 +610,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -626,7 +621,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -637,12 +632,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -653,7 +648,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -664,33 +659,34 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
-      <c r="C22">
+      <c r="B22">
         <v>0.8</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="B25">
+      <c r="B24">
         <v>5.7</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C24" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
langtjern parameter updates from GIS shp
</commit_message>
<xml_diff>
--- a/LangtjernLake/ConfigurationInputsLangtjern.xlsx
+++ b/LangtjernLake/ConfigurationInputsLangtjern.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Ian_GIS\gleon\SOS\LangtjernLake\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10110" windowHeight="4140"/>
   </bookViews>
@@ -436,7 +441,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -447,7 +452,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +478,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>32448</v>
+        <v>4221</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -495,7 +500,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>227000</v>
+        <v>224263</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
prop wetland canopy params
</commit_message>
<xml_diff>
--- a/LangtjernLake/ConfigurationInputsLangtjern.xlsx
+++ b/LangtjernLake/ConfigurationInputsLangtjern.xlsx
@@ -452,7 +452,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +565,7 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>0.65</v>
+        <v>0.71</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -576,7 +576,7 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>0.35</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>

</xml_diff>